<commit_message>
Vibration tests for ADXL1002
</commit_message>
<xml_diff>
--- a/uartFFTadc/SupportFilesADC/MEMS/ExperimentalData.xlsx
+++ b/uartFFTadc/SupportFilesADC/MEMS/ExperimentalData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\filestore.soton.ac.uk\users\tjg1g14\mydocuments\MScProject_EmbeddedSystems_ConditionMonitoring\uartFFTadc\SupportFiles\MEMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tim\Documents\GitHub\MScProject_EmbeddedSystems_ConditionMonitoring\uartFFTadc\SupportFilesADC\MEMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="13">
   <si>
     <t>Periodic Test</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>RMS Acc</t>
+  </si>
+  <si>
+    <t>ADXL1002</t>
   </si>
 </sst>
 </file>
@@ -1422,31 +1425,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:U32"/>
+  <dimension ref="B2:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27:I27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.26171875" customWidth="1"/>
+    <col min="4" max="4" width="12.26171875" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="Q3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1487,7 +1490,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -1528,7 +1531,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -1569,7 +1572,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -1595,7 +1598,7 @@
         <v>0.22589999999999999</v>
       </c>
     </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -1621,7 +1624,7 @@
         <v>0.24249999999999999</v>
       </c>
     </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -1647,7 +1650,7 @@
         <v>0.21310000000000001</v>
       </c>
     </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -1673,7 +1676,7 @@
         <v>0.24929999999999999</v>
       </c>
     </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -1699,7 +1702,7 @@
         <v>0.18970000000000001</v>
       </c>
     </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>0.2581</v>
       </c>
     </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
         <v>7</v>
       </c>
@@ -1751,7 +1754,7 @@
         <v>0.18870000000000001</v>
       </c>
     </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -1777,7 +1780,7 @@
         <v>0.27379999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -1803,7 +1806,7 @@
         <v>0.17499999999999999</v>
       </c>
     </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -1829,7 +1832,7 @@
         <v>0.28939999999999999</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -1855,7 +1858,7 @@
         <v>0.29330000000000001</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -1881,7 +1884,7 @@
         <v>0.40579999999999999</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
         <v>9</v>
       </c>
@@ -1907,7 +1910,7 @@
         <v>0.2276</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
         <v>9</v>
       </c>
@@ -1933,7 +1936,7 @@
         <v>0.20949999999999999</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" t="s">
         <v>9</v>
       </c>
@@ -1959,7 +1962,7 @@
         <v>0.38869999999999999</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B22" t="s">
         <v>9</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>0.41889999999999999</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
         <v>9</v>
       </c>
@@ -2011,7 +2014,7 @@
         <v>0.43509999999999999</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
         <v>9</v>
       </c>
@@ -2037,7 +2040,7 @@
         <v>0.53979999999999995</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
         <v>9</v>
       </c>
@@ -2063,7 +2066,7 @@
         <v>1.1641999999999999</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" t="s">
         <v>9</v>
       </c>
@@ -2089,7 +2092,7 @@
         <v>1.5025999999999999</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B27" t="s">
         <v>9</v>
       </c>
@@ -2115,7 +2118,7 @@
         <v>1.5125999999999999</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" t="s">
         <v>9</v>
       </c>
@@ -2141,7 +2144,7 @@
         <v>1.3292999999999999</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
         <v>9</v>
       </c>
@@ -2167,7 +2170,7 @@
         <v>1.1238999999999999</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" t="s">
         <v>9</v>
       </c>
@@ -2193,7 +2196,7 @@
         <v>1.6516</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" t="s">
         <v>9</v>
       </c>
@@ -2219,7 +2222,7 @@
         <v>0.27389999999999998</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B32" t="s">
         <v>9</v>
       </c>
@@ -2243,6 +2246,286 @@
       </c>
       <c r="I32">
         <v>0.43509999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <v>53</v>
+      </c>
+      <c r="D33">
+        <v>0.625</v>
+      </c>
+      <c r="E33">
+        <v>28</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34">
+        <v>95</v>
+      </c>
+      <c r="D34">
+        <v>1.25</v>
+      </c>
+      <c r="E34">
+        <v>27</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>553</v>
+      </c>
+      <c r="D35">
+        <v>3.1</v>
+      </c>
+      <c r="E35">
+        <v>56</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36">
+        <v>595</v>
+      </c>
+      <c r="D36">
+        <v>3.2</v>
+      </c>
+      <c r="E36">
+        <v>61</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <v>1053</v>
+      </c>
+      <c r="D37">
+        <v>6.1</v>
+      </c>
+      <c r="E37">
+        <v>75</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="G37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38">
+        <v>1095</v>
+      </c>
+      <c r="D38">
+        <v>6.2</v>
+      </c>
+      <c r="E38">
+        <v>96</v>
+      </c>
+      <c r="F38">
+        <v>2</v>
+      </c>
+      <c r="G38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39">
+        <v>1553</v>
+      </c>
+      <c r="D39">
+        <v>10.5</v>
+      </c>
+      <c r="E39">
+        <v>208</v>
+      </c>
+      <c r="F39">
+        <v>5</v>
+      </c>
+      <c r="G39">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40">
+        <v>1595</v>
+      </c>
+      <c r="D40">
+        <v>10.6</v>
+      </c>
+      <c r="E40">
+        <v>241</v>
+      </c>
+      <c r="F40">
+        <v>6</v>
+      </c>
+      <c r="G40">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41">
+        <v>2053</v>
+      </c>
+      <c r="D41">
+        <v>20</v>
+      </c>
+      <c r="E41">
+        <v>511</v>
+      </c>
+      <c r="F41">
+        <v>13</v>
+      </c>
+      <c r="G41">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42">
+        <v>2095</v>
+      </c>
+      <c r="D42">
+        <v>20</v>
+      </c>
+      <c r="E42">
+        <v>299</v>
+      </c>
+      <c r="F42">
+        <v>7</v>
+      </c>
+      <c r="G42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43">
+        <v>3053</v>
+      </c>
+      <c r="D43">
+        <v>20</v>
+      </c>
+      <c r="E43">
+        <v>714</v>
+      </c>
+      <c r="F43">
+        <v>22</v>
+      </c>
+      <c r="G43">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44">
+        <v>3095</v>
+      </c>
+      <c r="D44">
+        <v>20</v>
+      </c>
+      <c r="E44">
+        <v>1078</v>
+      </c>
+      <c r="F44">
+        <v>24</v>
+      </c>
+      <c r="G44">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45">
+        <v>4053</v>
+      </c>
+      <c r="D45">
+        <v>20</v>
+      </c>
+      <c r="E45">
+        <v>135</v>
+      </c>
+      <c r="F45">
+        <v>3</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46">
+        <v>4095</v>
+      </c>
+      <c r="D46">
+        <v>20</v>
+      </c>
+      <c r="E46">
+        <v>115</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>